<commit_message>
Added the research result from https://twitter.com/360bilalkhan/status/1588469937173336064 - https://docs.google.com/spreadsheets/d/1ttoxnh4GF6wKqV0dZR7CjvxY_05ZVBdpteHuUhsbwjQ/edit#gid=0
</commit_message>
<xml_diff>
--- a/evmos-private-sale.xlsx
+++ b/evmos-private-sale.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2700" windowWidth="28800" windowHeight="12570" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="28800" windowHeight="12570" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Unknown #2" sheetId="8" r:id="rId9"/>
     <sheet name="Unknown #3" sheetId="9" r:id="rId10"/>
     <sheet name="Unknown #4" sheetId="11" r:id="rId11"/>
+    <sheet name="360bilalkhan DATA" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="374">
   <si>
     <t>Name</t>
   </si>
@@ -896,6 +897,261 @@
   </si>
   <si>
     <t>Average Buying Price By Team Announcement Value 27M</t>
+  </si>
+  <si>
+    <t>Current Amount</t>
+  </si>
+  <si>
+    <t>Private Sale amount</t>
+  </si>
+  <si>
+    <t>3,900,000.00</t>
+  </si>
+  <si>
+    <t>3,315,233.41</t>
+  </si>
+  <si>
+    <t>2,700,000.00</t>
+  </si>
+  <si>
+    <t>2,507,334.93</t>
+  </si>
+  <si>
+    <t>1,650,000.00</t>
+  </si>
+  <si>
+    <t>174,472.95</t>
+  </si>
+  <si>
+    <t>142,105.26</t>
+  </si>
+  <si>
+    <t>131,469.30</t>
+  </si>
+  <si>
+    <t>86,842.10</t>
+  </si>
+  <si>
+    <t>205,263.16</t>
+  </si>
+  <si>
+    <t>Coinbase</t>
+  </si>
+  <si>
+    <t>5,543,021.35</t>
+  </si>
+  <si>
+    <t>4,800,000.00</t>
+  </si>
+  <si>
+    <t>291,713.10</t>
+  </si>
+  <si>
+    <t>252,630.58</t>
+  </si>
+  <si>
+    <t>194,377.60</t>
+  </si>
+  <si>
+    <t>175,438.60</t>
+  </si>
+  <si>
+    <t>194,384.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evmos1dlj5jmvf6g5e359hmsqlh6n0ce9j0kst7cwvp3 </t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>5263156.89</t>
+  </si>
+  <si>
+    <t>evmos1vltu2lkf9fhsm2dxhljhvaxcvwhzel5gaexrdu</t>
+  </si>
+  <si>
+    <t>1,892,846.83</t>
+  </si>
+  <si>
+    <t>evmos1yrnd07xnhghehqt26kqq6glmewvtslpcxqksr9</t>
+  </si>
+  <si>
+    <t>1,297,714.69</t>
+  </si>
+  <si>
+    <t>evmos1hnr9pchktsqtl9qea6z39kecwq2glcaxws0ver</t>
+  </si>
+  <si>
+    <t>1,570,307.30</t>
+  </si>
+  <si>
+    <t>evmos17hv5z07wed6yz52rt9dy3syleramp3w89n3h0g</t>
+  </si>
+  <si>
+    <t>325,780.14</t>
+  </si>
+  <si>
+    <t>evmos16dsetg9zr9g6q8lusk2xzkqqv4pnk4mquud8cr</t>
+  </si>
+  <si>
+    <t>403,251.89</t>
+  </si>
+  <si>
+    <t>Cosmostation VD</t>
+  </si>
+  <si>
+    <t>490,760.14</t>
+  </si>
+  <si>
+    <t>476,605.26</t>
+  </si>
+  <si>
+    <t>84,561.66</t>
+  </si>
+  <si>
+    <t>84,210.53</t>
+  </si>
+  <si>
+    <t>Chrous One</t>
+  </si>
+  <si>
+    <t>105,276.11</t>
+  </si>
+  <si>
+    <t>Informal</t>
+  </si>
+  <si>
+    <t>37,847.21</t>
+  </si>
+  <si>
+    <t>36,842.11</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>1,950,000.00</t>
+  </si>
+  <si>
+    <t>1,949,998.99</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>102,631.58</t>
+  </si>
+  <si>
+    <t>evmos1y22k2wu0fvt3epz3tzl6wh09wu8f5wtughfjy3</t>
+  </si>
+  <si>
+    <t>102,630.57</t>
+  </si>
+  <si>
+    <t>beehive</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1vpvzta06qecq9w0gn427u8zd02cpk2rhak8t57</t>
+  </si>
+  <si>
+    <t>105,262.16</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos15em5an445cqrcqxh2a9lw0w8dm44vt4tgdk8g2</t>
+  </si>
+  <si>
+    <t>73,683.21</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos19pvfc52dsc7vv8uvkgcnnfxj5t3hrnvpvfkjkh</t>
+  </si>
+  <si>
+    <t>10,525.32</t>
+  </si>
+  <si>
+    <t>unidentifiable</t>
+  </si>
+  <si>
+    <t>1,578,947.37</t>
+  </si>
+  <si>
+    <t>1,052,631.58</t>
+  </si>
+  <si>
+    <t>154,976.77</t>
+  </si>
+  <si>
+    <t>154,974.68</t>
+  </si>
+  <si>
+    <t>25,257,903.70</t>
+  </si>
+  <si>
+    <t>Unconfirmed</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1tu7y6yh6zj5nev95gffuadydxfxwwx7ac6fxuw</t>
+  </si>
+  <si>
+    <t>42,105.26</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1vnjx6u8c2akepmzsncvqdrmntzg385z5jxjppp</t>
+  </si>
+  <si>
+    <t>10,526.32</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos10kwhxnv7gttzlnlvj25u8rqancnqdlga405585</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1g0ftmg9u37hmdkjtudsdmvmqquuzecrwk3nuzx</t>
+  </si>
+  <si>
+    <t>63,157.89</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1sxttkjsmt9eht4xry6hc4u58xc7gyys4qhn9td</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1zdps32zqxqk4t6e3msf2zmmf2vp3tkwcyk5zh7</t>
+  </si>
+  <si>
+    <t>5,263.16</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1lcv8ddm4yefl8qxsdaeazcddmuclqxx0j22cjx</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1wmur7246ffqgt2rlhedukdq3cpy7l3df0ds8yr</t>
+  </si>
+  <si>
+    <t>26,315.79</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1t9kny6qmp26y62tty5cveslk89qx4542wm624g</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1yusd9sxux5z7gn8gkakj0d7sddktp9ynhmry0u</t>
+  </si>
+  <si>
+    <t>263,157.89</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1uwgf5kh2sqy2qwudvngwk6yuemf57w3w4xun59</t>
+  </si>
+  <si>
+    <t>21,052.63</t>
+  </si>
+  <si>
+    <t>https://www.mintscan.io/evmos/account/evmos1rmrye8pkvq9dscqp7jh299q87dzc29tysvszzf</t>
+  </si>
+  <si>
+    <t>25,826,324.75</t>
   </si>
 </sst>
 </file>
@@ -12084,7 +12340,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12621,6 +12877,502 @@
       </c>
       <c r="F2" s="4">
         <v>44918.736018518517</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="90.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>306</v>
+      </c>
+      <c r="C13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>309</v>
+      </c>
+      <c r="B16" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>314</v>
+      </c>
+      <c r="B18" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>318</v>
+      </c>
+      <c r="B20" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>320</v>
+      </c>
+      <c r="B21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" t="s">
+        <v>323</v>
+      </c>
+      <c r="C23" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
+        <v>325</v>
+      </c>
+      <c r="C24" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B28" t="s">
+        <v>328</v>
+      </c>
+      <c r="C28" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" t="s">
+        <v>330</v>
+      </c>
+      <c r="C30" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>333</v>
+      </c>
+      <c r="C32" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>336</v>
+      </c>
+      <c r="C34" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>338</v>
+      </c>
+      <c r="B35" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>341</v>
+      </c>
+      <c r="C37" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>343</v>
+      </c>
+      <c r="C38" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>345</v>
+      </c>
+      <c r="C39" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
+        <v>348</v>
+      </c>
+      <c r="C41" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" t="s">
+        <v>349</v>
+      </c>
+      <c r="C42" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>129</v>
+      </c>
+      <c r="B43" t="s">
+        <v>350</v>
+      </c>
+      <c r="C43" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>354</v>
+      </c>
+      <c r="C50" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>356</v>
+      </c>
+      <c r="C51" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>358</v>
+      </c>
+      <c r="C52" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>359</v>
+      </c>
+      <c r="C53" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>361</v>
+      </c>
+      <c r="C54" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>362</v>
+      </c>
+      <c r="C55" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>364</v>
+      </c>
+      <c r="C56" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>365</v>
+      </c>
+      <c r="C57" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>367</v>
+      </c>
+      <c r="C58" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>368</v>
+      </c>
+      <c r="C59" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>370</v>
+      </c>
+      <c r="C60" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>372</v>
+      </c>
+      <c r="C61" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -17096,7 +17848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AD10" sqref="AD10"/>
     </sheetView>
   </sheetViews>

</xml_diff>